<commit_message>
Posting multiple products at a time and selecting any one of them
</commit_message>
<xml_diff>
--- a/Data for POST.xlsx
+++ b/Data for POST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbalsaraf\API_CRUD\REST_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27506D57-9168-41ED-BB39-64753245C1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0881E0F9-834C-405A-A89A-F9F162B8F7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2359DD1B-B355-424D-8F6D-E419607D45CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>1TB</t>
+  </si>
+  <si>
+    <t>iPhone 17</t>
+  </si>
+  <si>
+    <t>2TB</t>
+  </si>
+  <si>
+    <t>One plus 5</t>
+  </si>
+  <si>
+    <t>i5</t>
+  </si>
+  <si>
+    <t>4GB</t>
   </si>
 </sst>
 </file>
@@ -431,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED86EBD-D180-401E-B2B7-B8C03FC1FAE5}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,6 +495,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2025</v>
+      </c>
+      <c r="C3">
+        <v>120000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2023</v>
+      </c>
+      <c r="C4">
+        <v>70000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>